<commit_message>
Added notes of graphs in report
methodology section
> Graphs
> Analysation notes
</commit_message>
<xml_diff>
--- a/preformance logs/Vectors/features/Performance Logs.xlsx
+++ b/preformance logs/Vectors/features/Performance Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pana\Desktop\Northumbria\Final Year\Individual Computing Project KV6003BNN01\Speech-Emotion-Recognition---Audio-Dataset\preformance logs\Vectors\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57339BE2-AE7B-4B93-85C8-7457E5C8B420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45271BD-C4EB-4306-B182-0D0791E2908B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{61528B2F-A6A9-4B14-924A-8C83E0EA857F}"/>
   </bookViews>
@@ -514,15 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,12 +521,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -554,6 +539,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1906,11 +1906,11 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> DATASETS</a:t>
+              <a:t> DATASETS - VECTOR FEATURES</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>: Mel-Spectrogram vs MFCC</a:t>
+              <a:t>:    Mel-Spectrogram vs MFCC</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2866,7 +2866,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>MACHINE LEARNING - ALL DATASETS : Mel-Spectrogram vs MFCC</a:t>
+              <a:t>MACHINE LEARNING - ALL DATASETS - VECTOR FEATURES: Mel-Spectrogram vs MFCC</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -31030,8 +31030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E156107A-CEDE-4609-AC71-C70C41097B85}">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AB62" activeCellId="1" sqref="Z62:Z66 AB62:AB66"/>
+    <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Z66" sqref="Z5:AC66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31044,69 +31044,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="29"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="24"/>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="32"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="27"/>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -31170,46 +31170,46 @@
       <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="K5" s="19" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="K5" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="21"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="21"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="30"/>
       <c r="T5" s="16"/>
-      <c r="U5" s="19" t="s">
+      <c r="U5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="21"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="30"/>
       <c r="Y5" s="16"/>
-      <c r="Z5" s="19" t="s">
+      <c r="Z5" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="21"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="30"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -31694,33 +31694,33 @@
       <c r="I12" s="9">
         <v>0.37</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="22" t="s">
+      <c r="P12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="24"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="21"/>
       <c r="T12" s="16"/>
-      <c r="U12" s="22" t="s">
+      <c r="U12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="24"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="21"/>
       <c r="Y12" s="16"/>
-      <c r="Z12" s="22" t="s">
+      <c r="Z12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="24"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="21"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -32211,46 +32211,46 @@
       <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="K21" s="19" t="s">
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="K21" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="21"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="21"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="30"/>
       <c r="T21" s="16"/>
-      <c r="U21" s="19" t="s">
+      <c r="U21" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="V21" s="20"/>
-      <c r="W21" s="20"/>
-      <c r="X21" s="21"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="30"/>
       <c r="Y21" s="16"/>
-      <c r="Z21" s="19" t="s">
+      <c r="Z21" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="AA21" s="20"/>
-      <c r="AB21" s="20"/>
-      <c r="AC21" s="21"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="30"/>
     </row>
     <row r="22" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -32734,33 +32734,33 @@
       <c r="I28" s="9">
         <v>0.24</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="24"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="21"/>
       <c r="O28" s="16"/>
-      <c r="P28" s="22" t="s">
+      <c r="P28" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="24"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="21"/>
       <c r="T28" s="16"/>
-      <c r="U28" s="22" t="s">
+      <c r="U28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="24"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="21"/>
       <c r="Y28" s="16"/>
-      <c r="Z28" s="22" t="s">
+      <c r="Z28" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="AA28" s="23"/>
-      <c r="AB28" s="23"/>
-      <c r="AC28" s="24"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="21"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -33251,46 +33251,46 @@
       <c r="AC36" s="14"/>
     </row>
     <row r="37" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="16"/>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="24"/>
-      <c r="K37" s="19" t="s">
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="21"/>
+      <c r="K37" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="21"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="30"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="19" t="s">
+      <c r="P37" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="21"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="30"/>
       <c r="T37" s="16"/>
-      <c r="U37" s="19" t="s">
+      <c r="U37" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="21"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="30"/>
       <c r="Y37" s="16"/>
-      <c r="Z37" s="19" t="s">
+      <c r="Z37" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="21"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="30"/>
     </row>
     <row r="38" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -33774,33 +33774,33 @@
       <c r="I44" s="9">
         <v>0.21</v>
       </c>
-      <c r="K44" s="22" t="s">
+      <c r="K44" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="24"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="21"/>
       <c r="O44" s="16"/>
-      <c r="P44" s="22" t="s">
+      <c r="P44" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="24"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="21"/>
       <c r="T44" s="16"/>
-      <c r="U44" s="22" t="s">
+      <c r="U44" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="24"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="21"/>
       <c r="Y44" s="16"/>
-      <c r="Z44" s="22" t="s">
+      <c r="Z44" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="AA44" s="23"/>
-      <c r="AB44" s="23"/>
-      <c r="AC44" s="24"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="21"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -34291,46 +34291,46 @@
       <c r="AC52" s="14"/>
     </row>
     <row r="53" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="16"/>
-      <c r="F53" s="22" t="s">
+      <c r="F53" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="24"/>
-      <c r="K53" s="19" t="s">
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="21"/>
+      <c r="K53" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="21"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="30"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="19" t="s">
+      <c r="P53" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="21"/>
+      <c r="Q53" s="29"/>
+      <c r="R53" s="29"/>
+      <c r="S53" s="30"/>
       <c r="T53" s="16"/>
-      <c r="U53" s="19" t="s">
+      <c r="U53" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="V53" s="20"/>
-      <c r="W53" s="20"/>
-      <c r="X53" s="21"/>
+      <c r="V53" s="29"/>
+      <c r="W53" s="29"/>
+      <c r="X53" s="30"/>
       <c r="Y53" s="16"/>
-      <c r="Z53" s="19" t="s">
+      <c r="Z53" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="AA53" s="20"/>
-      <c r="AB53" s="20"/>
-      <c r="AC53" s="21"/>
+      <c r="AA53" s="29"/>
+      <c r="AB53" s="29"/>
+      <c r="AC53" s="30"/>
     </row>
     <row r="54" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -34814,33 +34814,33 @@
       <c r="I60" s="9">
         <v>0.26</v>
       </c>
-      <c r="K60" s="22" t="s">
+      <c r="K60" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="L60" s="23"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="24"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="21"/>
       <c r="O60" s="16"/>
-      <c r="P60" s="22" t="s">
+      <c r="P60" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="23"/>
-      <c r="S60" s="24"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="21"/>
       <c r="T60" s="16"/>
-      <c r="U60" s="22" t="s">
+      <c r="U60" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="V60" s="23"/>
-      <c r="W60" s="23"/>
-      <c r="X60" s="24"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+      <c r="X60" s="21"/>
       <c r="Y60" s="16"/>
-      <c r="Z60" s="22" t="s">
+      <c r="Z60" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AA60" s="23"/>
-      <c r="AB60" s="23"/>
-      <c r="AC60" s="24"/>
+      <c r="AA60" s="20"/>
+      <c r="AB60" s="20"/>
+      <c r="AC60" s="21"/>
     </row>
     <row r="61" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -35332,6 +35332,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="P53:S53"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="P21:S21"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="U53:X53"/>
+    <mergeCell ref="Z53:AC53"/>
+    <mergeCell ref="U60:X60"/>
+    <mergeCell ref="Z60:AC60"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="P37:S37"/>
+    <mergeCell ref="K53:N53"/>
     <mergeCell ref="K60:N60"/>
     <mergeCell ref="P28:S28"/>
     <mergeCell ref="K1:AC2"/>
@@ -35348,32 +35374,6 @@
     <mergeCell ref="P60:S60"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U53:X53"/>
-    <mergeCell ref="Z53:AC53"/>
-    <mergeCell ref="U60:X60"/>
-    <mergeCell ref="Z60:AC60"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="P37:S37"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="P53:S53"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="P21:S21"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="P44:S44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -35384,8 +35384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FD7A86-73DA-44B2-B0E2-52543668D857}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView topLeftCell="H13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ23" sqref="AJ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35399,8 +35399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122FAC1-14A9-4631-87C8-BC63A01CE8FE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O64" sqref="O64"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CY36" sqref="CY36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Image Creation + GenAlg Updates
</commit_message>
<xml_diff>
--- a/preformance logs/Vectors/features/Performance Logs.xlsx
+++ b/preformance logs/Vectors/features/Performance Logs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pana\Desktop\Northumbria\Final Year\Individual Computing Project KV6003BNN01\Speech-Emotion-Recognition---Audio-Dataset\preformance logs\Vectors\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E00D15-977C-4946-AF20-964B2823C771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B26EE43-642A-4C29-89CA-1125ADD888F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{61528B2F-A6A9-4B14-924A-8C83E0EA857F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="66">
   <si>
     <t>ANN</t>
   </si>
@@ -213,6 +213,30 @@
   <si>
     <t>SAVEE: MFCC  256X256</t>
   </si>
+  <si>
+    <t>3 Channel Feature EMODB Dataset</t>
+  </si>
+  <si>
+    <t>Vector Features - Gen Alg Optimisation</t>
+  </si>
+  <si>
+    <t>CH_ME_MF</t>
+  </si>
+  <si>
+    <t>CH_MF_ME</t>
+  </si>
+  <si>
+    <t>MF_CH_ME</t>
+  </si>
+  <si>
+    <t>MF_ME_CH</t>
+  </si>
+  <si>
+    <t>ME_CH_MF</t>
+  </si>
+  <si>
+    <t>ME_MF_CH</t>
+  </si>
 </sst>
 </file>
 
@@ -258,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +346,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9393"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5757"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -514,15 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,12 +569,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -556,6 +589,48 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,16 +639,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5757"/>
+      <color rgb="FFFF9393"/>
+      <color rgb="FFFF8989"/>
+      <color rgb="FFFFD3D3"/>
+      <color rgb="FFFF7979"/>
       <color rgb="FFEC7014"/>
       <color rgb="FFCB181D"/>
       <color rgb="FF238B45"/>
       <color rgb="FF2171B5"/>
       <color rgb="FFFD9351"/>
-      <color rgb="FFFB6A4A"/>
-      <color rgb="FF74C476"/>
-      <color rgb="FF6BAED6"/>
-      <color rgb="FFFF7979"/>
-      <color rgb="FFFEC49F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -31028,10 +31103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E156107A-CEDE-4609-AC71-C70C41097B85}">
-  <dimension ref="A1:AC68"/>
+  <dimension ref="A1:AM68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AL105" sqref="AL105"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31041,74 +31116,96 @@
     <col min="6" max="14" width="18.5703125" customWidth="1"/>
     <col min="15" max="15" width="17.5703125" customWidth="1"/>
     <col min="16" max="29" width="18.5703125" customWidth="1"/>
+    <col min="30" max="30" width="25.5703125" customWidth="1"/>
+    <col min="31" max="34" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="29"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="24"/>
+      <c r="AE1" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
     </row>
-    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="32"/>
+    <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="27"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
     </row>
-    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -31139,7 +31236,7 @@
       <c r="AB3" s="16"/>
       <c r="AC3" s="14"/>
     </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -31169,49 +31266,55 @@
       <c r="AB4" s="16"/>
       <c r="AC4" s="14"/>
     </row>
-    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="K5" s="19" t="s">
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="K5" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="21"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="21"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="30"/>
       <c r="T5" s="16"/>
-      <c r="U5" s="19" t="s">
+      <c r="U5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="21"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="30"/>
       <c r="Y5" s="16"/>
-      <c r="Z5" s="19" t="s">
+      <c r="Z5" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="21"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="30"/>
+      <c r="AE5" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF5" s="41"/>
+      <c r="AG5" s="41"/>
+      <c r="AH5" s="41"/>
     </row>
-    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -31276,8 +31379,18 @@
       <c r="AC6" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG6" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH6" s="38" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -31354,8 +31467,20 @@
       <c r="AC7" s="10">
         <v>0.51</v>
       </c>
+      <c r="AE7" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF7" s="34">
+        <v>0.79</v>
+      </c>
+      <c r="AG7" s="35">
+        <v>0.73</v>
+      </c>
+      <c r="AH7" s="34">
+        <v>0.79</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -31432,8 +31557,20 @@
       <c r="AC8" s="10">
         <v>0.49</v>
       </c>
+      <c r="AE8" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF8" s="34">
+        <v>0.78</v>
+      </c>
+      <c r="AG8" s="35">
+        <v>0.7</v>
+      </c>
+      <c r="AH8" s="34">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -31511,8 +31648,20 @@
       <c r="AC9" s="10">
         <v>0.5</v>
       </c>
+      <c r="AE9" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF9" s="34">
+        <v>0.81</v>
+      </c>
+      <c r="AG9" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="AH9" s="34">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -31589,8 +31738,20 @@
       <c r="AC10" s="10">
         <v>0.57999999999999996</v>
       </c>
+      <c r="AE10" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF10" s="34">
+        <v>0.79</v>
+      </c>
+      <c r="AG10" s="35">
+        <v>0.69</v>
+      </c>
+      <c r="AH10" s="34">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -31667,8 +31828,20 @@
       <c r="AC11" s="10">
         <v>0.49</v>
       </c>
+      <c r="AE11" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF11" s="34">
+        <v>0.74</v>
+      </c>
+      <c r="AG11" s="35">
+        <v>0.66</v>
+      </c>
+      <c r="AH11" s="34">
+        <v>0.73</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -31694,35 +31867,41 @@
       <c r="I12" s="9">
         <v>0.37</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="22" t="s">
+      <c r="P12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="24"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="21"/>
       <c r="T12" s="16"/>
-      <c r="U12" s="22" t="s">
+      <c r="U12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="24"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="21"/>
       <c r="Y12" s="16"/>
-      <c r="Z12" s="22" t="s">
+      <c r="Z12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="24"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="21"/>
+      <c r="AE12" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF12" s="34"/>
+      <c r="AG12" s="35"/>
+      <c r="AH12" s="34"/>
     </row>
-    <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -31791,8 +31970,12 @@
       <c r="AC13" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="AE13" s="39"/>
+      <c r="AF13" s="40"/>
+      <c r="AG13" s="40"/>
+      <c r="AH13" s="40"/>
     </row>
-    <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -31869,8 +32052,12 @@
       <c r="AC14" s="9">
         <v>0.04</v>
       </c>
+      <c r="AE14" s="39"/>
+      <c r="AF14" s="40"/>
+      <c r="AG14" s="40"/>
+      <c r="AH14" s="40"/>
     </row>
-    <row r="15" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -31947,8 +32134,12 @@
       <c r="AC15" s="9">
         <v>0.43</v>
       </c>
+      <c r="AE15" s="39"/>
+      <c r="AF15" s="40"/>
+      <c r="AG15" s="40"/>
+      <c r="AH15" s="40"/>
     </row>
-    <row r="16" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -32025,6 +32216,10 @@
       <c r="AC16" s="9">
         <v>0.4</v>
       </c>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="40"/>
+      <c r="AG16" s="40"/>
+      <c r="AH16" s="40"/>
     </row>
     <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
@@ -32211,46 +32406,46 @@
       <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="K21" s="19" t="s">
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="K21" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="21"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="21"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="30"/>
       <c r="T21" s="16"/>
-      <c r="U21" s="19" t="s">
+      <c r="U21" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="V21" s="20"/>
-      <c r="W21" s="20"/>
-      <c r="X21" s="21"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="30"/>
       <c r="Y21" s="16"/>
-      <c r="Z21" s="19" t="s">
+      <c r="Z21" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="AA21" s="20"/>
-      <c r="AB21" s="20"/>
-      <c r="AC21" s="21"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="30"/>
     </row>
     <row r="22" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -32734,33 +32929,33 @@
       <c r="I28" s="9">
         <v>0.24</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="24"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="21"/>
       <c r="O28" s="16"/>
-      <c r="P28" s="22" t="s">
+      <c r="P28" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="24"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="21"/>
       <c r="T28" s="16"/>
-      <c r="U28" s="22" t="s">
+      <c r="U28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="24"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="21"/>
       <c r="Y28" s="16"/>
-      <c r="Z28" s="22" t="s">
+      <c r="Z28" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="AA28" s="23"/>
-      <c r="AB28" s="23"/>
-      <c r="AC28" s="24"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="21"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -33251,46 +33446,46 @@
       <c r="AC36" s="14"/>
     </row>
     <row r="37" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="16"/>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="24"/>
-      <c r="K37" s="19" t="s">
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="21"/>
+      <c r="K37" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="21"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="30"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="19" t="s">
+      <c r="P37" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="21"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="30"/>
       <c r="T37" s="16"/>
-      <c r="U37" s="19" t="s">
+      <c r="U37" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="21"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="30"/>
       <c r="Y37" s="16"/>
-      <c r="Z37" s="19" t="s">
+      <c r="Z37" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="21"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="30"/>
     </row>
     <row r="38" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -33774,33 +33969,33 @@
       <c r="I44" s="9">
         <v>0.21</v>
       </c>
-      <c r="K44" s="22" t="s">
+      <c r="K44" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="24"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="21"/>
       <c r="O44" s="16"/>
-      <c r="P44" s="22" t="s">
+      <c r="P44" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="24"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="21"/>
       <c r="T44" s="16"/>
-      <c r="U44" s="22" t="s">
+      <c r="U44" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="24"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="21"/>
       <c r="Y44" s="16"/>
-      <c r="Z44" s="22" t="s">
+      <c r="Z44" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="AA44" s="23"/>
-      <c r="AB44" s="23"/>
-      <c r="AC44" s="24"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="21"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -34291,46 +34486,46 @@
       <c r="AC52" s="14"/>
     </row>
     <row r="53" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="16"/>
-      <c r="F53" s="22" t="s">
+      <c r="F53" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="24"/>
-      <c r="K53" s="19" t="s">
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="21"/>
+      <c r="K53" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="21"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="30"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="19" t="s">
+      <c r="P53" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="21"/>
+      <c r="Q53" s="29"/>
+      <c r="R53" s="29"/>
+      <c r="S53" s="30"/>
       <c r="T53" s="16"/>
-      <c r="U53" s="19" t="s">
+      <c r="U53" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="V53" s="20"/>
-      <c r="W53" s="20"/>
-      <c r="X53" s="21"/>
+      <c r="V53" s="29"/>
+      <c r="W53" s="29"/>
+      <c r="X53" s="30"/>
       <c r="Y53" s="16"/>
-      <c r="Z53" s="19" t="s">
+      <c r="Z53" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="AA53" s="20"/>
-      <c r="AB53" s="20"/>
-      <c r="AC53" s="21"/>
+      <c r="AA53" s="29"/>
+      <c r="AB53" s="29"/>
+      <c r="AC53" s="30"/>
     </row>
     <row r="54" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -34814,33 +35009,33 @@
       <c r="I60" s="9">
         <v>0.26</v>
       </c>
-      <c r="K60" s="22" t="s">
+      <c r="K60" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="L60" s="23"/>
-      <c r="M60" s="23"/>
-      <c r="N60" s="24"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="21"/>
       <c r="O60" s="16"/>
-      <c r="P60" s="22" t="s">
+      <c r="P60" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="23"/>
-      <c r="S60" s="24"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="21"/>
       <c r="T60" s="16"/>
-      <c r="U60" s="22" t="s">
+      <c r="U60" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="V60" s="23"/>
-      <c r="W60" s="23"/>
-      <c r="X60" s="24"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+      <c r="X60" s="21"/>
       <c r="Y60" s="16"/>
-      <c r="Z60" s="22" t="s">
+      <c r="Z60" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="AA60" s="23"/>
-      <c r="AB60" s="23"/>
-      <c r="AC60" s="24"/>
+      <c r="AA60" s="20"/>
+      <c r="AB60" s="20"/>
+      <c r="AC60" s="21"/>
     </row>
     <row r="61" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -35331,7 +35526,35 @@
       <c r="AC68" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="44">
+    <mergeCell ref="AE5:AH5"/>
+    <mergeCell ref="AE1:AH2"/>
+    <mergeCell ref="P53:S53"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="P21:S21"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="U53:X53"/>
+    <mergeCell ref="Z53:AC53"/>
+    <mergeCell ref="U60:X60"/>
+    <mergeCell ref="Z60:AC60"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="P37:S37"/>
+    <mergeCell ref="K53:N53"/>
     <mergeCell ref="K60:N60"/>
     <mergeCell ref="P28:S28"/>
     <mergeCell ref="K1:AC2"/>
@@ -35348,32 +35571,6 @@
     <mergeCell ref="P60:S60"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U53:X53"/>
-    <mergeCell ref="Z53:AC53"/>
-    <mergeCell ref="U60:X60"/>
-    <mergeCell ref="Z60:AC60"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="P37:S37"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="P53:S53"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="P21:S21"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="P44:S44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Overnight Execution of GenAlg
Created multiple instances of the same Genetic Algorithm for the RAVDESS dataset, that I need to test 6 times from different image datasets of it. The process will take long hours to finish, thus I have this to run during the night
</commit_message>
<xml_diff>
--- a/preformance logs/Vectors/features/Performance Logs.xlsx
+++ b/preformance logs/Vectors/features/Performance Logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pana\Desktop\Northumbria\Final Year\Individual Computing Project KV6003BNN01\Speech-Emotion-Recognition---Audio-Dataset\preformance logs\Vectors\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B26EE43-642A-4C29-89CA-1125ADD888F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3BE333-A801-4512-9584-EEDC9C03A0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{61528B2F-A6A9-4B14-924A-8C83E0EA857F}"/>
+    <workbookView xWindow="7200" yWindow="1620" windowWidth="21600" windowHeight="11835" xr2:uid="{61528B2F-A6A9-4B14-924A-8C83E0EA857F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -562,6 +562,45 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,6 +608,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -587,48 +629,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -31105,8 +31105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E156107A-CEDE-4609-AC71-C70C41097B85}">
   <dimension ref="A1:AM68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AI12" sqref="AI12"/>
+    <sheetView tabSelected="1" topLeftCell="AD4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31121,89 +31121,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="24"/>
-      <c r="AE1" s="31" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="38"/>
+      <c r="AE1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="27"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="41"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -31267,52 +31267,52 @@
       <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="K5" s="28" t="s">
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="K5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="31"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="16"/>
-      <c r="U5" s="28" t="s">
+      <c r="U5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="31"/>
       <c r="Y5" s="16"/>
-      <c r="Z5" s="28" t="s">
+      <c r="Z5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="30"/>
-      <c r="AE5" s="41" t="s">
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="31"/>
+      <c r="AE5" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="AF5" s="41"/>
-      <c r="AG5" s="41"/>
-      <c r="AH5" s="41"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
     </row>
     <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -31379,14 +31379,14 @@
       <c r="AC6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AE6" s="36"/>
-      <c r="AF6" s="38" t="s">
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="AG6" s="38" t="s">
+      <c r="AG6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AH6" s="38" t="s">
+      <c r="AH6" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -31467,16 +31467,16 @@
       <c r="AC7" s="10">
         <v>0.51</v>
       </c>
-      <c r="AE7" s="37" t="s">
+      <c r="AE7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AF7" s="34">
+      <c r="AF7" s="20">
         <v>0.79</v>
       </c>
-      <c r="AG7" s="35">
+      <c r="AG7" s="21">
         <v>0.73</v>
       </c>
-      <c r="AH7" s="34">
+      <c r="AH7" s="20">
         <v>0.79</v>
       </c>
     </row>
@@ -31557,16 +31557,16 @@
       <c r="AC8" s="10">
         <v>0.49</v>
       </c>
-      <c r="AE8" s="37" t="s">
+      <c r="AE8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="AF8" s="34">
+      <c r="AF8" s="20">
         <v>0.78</v>
       </c>
-      <c r="AG8" s="35">
+      <c r="AG8" s="21">
         <v>0.7</v>
       </c>
-      <c r="AH8" s="34">
+      <c r="AH8" s="20">
         <v>0.77</v>
       </c>
     </row>
@@ -31648,16 +31648,16 @@
       <c r="AC9" s="10">
         <v>0.5</v>
       </c>
-      <c r="AE9" s="37" t="s">
+      <c r="AE9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="AF9" s="34">
+      <c r="AF9" s="20">
         <v>0.81</v>
       </c>
-      <c r="AG9" s="35">
+      <c r="AG9" s="21">
         <v>0.75</v>
       </c>
-      <c r="AH9" s="34">
+      <c r="AH9" s="20">
         <v>0.81</v>
       </c>
     </row>
@@ -31738,16 +31738,16 @@
       <c r="AC10" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AE10" s="37" t="s">
+      <c r="AE10" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="AF10" s="34">
+      <c r="AF10" s="20">
         <v>0.79</v>
       </c>
-      <c r="AG10" s="35">
+      <c r="AG10" s="21">
         <v>0.69</v>
       </c>
-      <c r="AH10" s="34">
+      <c r="AH10" s="20">
         <v>0.77</v>
       </c>
     </row>
@@ -31828,16 +31828,16 @@
       <c r="AC11" s="10">
         <v>0.49</v>
       </c>
-      <c r="AE11" s="37" t="s">
+      <c r="AE11" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="AF11" s="34">
+      <c r="AF11" s="20">
         <v>0.74</v>
       </c>
-      <c r="AG11" s="35">
+      <c r="AG11" s="21">
         <v>0.66</v>
       </c>
-      <c r="AH11" s="34">
+      <c r="AH11" s="20">
         <v>0.73</v>
       </c>
     </row>
@@ -31867,39 +31867,45 @@
       <c r="I12" s="9">
         <v>0.37</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="21"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="19" t="s">
+      <c r="P12" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="21"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="34"/>
       <c r="T12" s="16"/>
-      <c r="U12" s="19" t="s">
+      <c r="U12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="21"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="34"/>
       <c r="Y12" s="16"/>
-      <c r="Z12" s="19" t="s">
+      <c r="Z12" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="AA12" s="20"/>
-      <c r="AB12" s="20"/>
-      <c r="AC12" s="21"/>
-      <c r="AE12" s="37" t="s">
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="34"/>
+      <c r="AE12" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="AF12" s="34"/>
-      <c r="AG12" s="35"/>
-      <c r="AH12" s="34"/>
+      <c r="AF12" s="20">
+        <v>0.81</v>
+      </c>
+      <c r="AG12" s="21">
+        <v>0.74</v>
+      </c>
+      <c r="AH12" s="20">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -31970,10 +31976,10 @@
       <c r="AC13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AE13" s="39"/>
-      <c r="AF13" s="40"/>
-      <c r="AG13" s="40"/>
-      <c r="AH13" s="40"/>
+      <c r="AE13" s="25"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
     </row>
     <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -32052,10 +32058,10 @@
       <c r="AC14" s="9">
         <v>0.04</v>
       </c>
-      <c r="AE14" s="39"/>
-      <c r="AF14" s="40"/>
-      <c r="AG14" s="40"/>
-      <c r="AH14" s="40"/>
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
     </row>
     <row r="15" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -32134,10 +32140,10 @@
       <c r="AC15" s="9">
         <v>0.43</v>
       </c>
-      <c r="AE15" s="39"/>
-      <c r="AF15" s="40"/>
-      <c r="AG15" s="40"/>
-      <c r="AH15" s="40"/>
+      <c r="AE15" s="25"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
     </row>
     <row r="16" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -32216,10 +32222,10 @@
       <c r="AC16" s="9">
         <v>0.4</v>
       </c>
-      <c r="AE16" s="39"/>
-      <c r="AF16" s="40"/>
-      <c r="AG16" s="40"/>
-      <c r="AH16" s="40"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="26"/>
+      <c r="AG16" s="26"/>
+      <c r="AH16" s="26"/>
     </row>
     <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
@@ -32406,46 +32412,46 @@
       <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-      <c r="K21" s="28" t="s">
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+      <c r="K21" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="28" t="s">
+      <c r="P21" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="31"/>
       <c r="T21" s="16"/>
-      <c r="U21" s="28" t="s">
+      <c r="U21" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="31"/>
       <c r="Y21" s="16"/>
-      <c r="Z21" s="28" t="s">
+      <c r="Z21" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="AA21" s="29"/>
-      <c r="AB21" s="29"/>
-      <c r="AC21" s="30"/>
+      <c r="AA21" s="30"/>
+      <c r="AB21" s="30"/>
+      <c r="AC21" s="31"/>
     </row>
     <row r="22" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -32929,33 +32935,33 @@
       <c r="I28" s="9">
         <v>0.24</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="21"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="34"/>
       <c r="O28" s="16"/>
-      <c r="P28" s="19" t="s">
+      <c r="P28" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="21"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="34"/>
       <c r="T28" s="16"/>
-      <c r="U28" s="19" t="s">
+      <c r="U28" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="21"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
+      <c r="X28" s="34"/>
       <c r="Y28" s="16"/>
-      <c r="Z28" s="19" t="s">
+      <c r="Z28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AC28" s="21"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="34"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -33446,46 +33452,46 @@
       <c r="AC36" s="14"/>
     </row>
     <row r="37" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="16"/>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="21"/>
-      <c r="K37" s="28" t="s">
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="34"/>
+      <c r="K37" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="30"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="31"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="28" t="s">
+      <c r="P37" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="30"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="31"/>
       <c r="T37" s="16"/>
-      <c r="U37" s="28" t="s">
+      <c r="U37" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="30"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
+      <c r="X37" s="31"/>
       <c r="Y37" s="16"/>
-      <c r="Z37" s="28" t="s">
+      <c r="Z37" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AA37" s="29"/>
-      <c r="AB37" s="29"/>
-      <c r="AC37" s="30"/>
+      <c r="AA37" s="30"/>
+      <c r="AB37" s="30"/>
+      <c r="AC37" s="31"/>
     </row>
     <row r="38" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -33969,33 +33975,33 @@
       <c r="I44" s="9">
         <v>0.21</v>
       </c>
-      <c r="K44" s="19" t="s">
+      <c r="K44" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="21"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="34"/>
       <c r="O44" s="16"/>
-      <c r="P44" s="19" t="s">
+      <c r="P44" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="21"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="33"/>
+      <c r="S44" s="34"/>
       <c r="T44" s="16"/>
-      <c r="U44" s="19" t="s">
+      <c r="U44" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="21"/>
+      <c r="V44" s="33"/>
+      <c r="W44" s="33"/>
+      <c r="X44" s="34"/>
       <c r="Y44" s="16"/>
-      <c r="Z44" s="19" t="s">
+      <c r="Z44" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="AA44" s="20"/>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="21"/>
+      <c r="AA44" s="33"/>
+      <c r="AB44" s="33"/>
+      <c r="AC44" s="34"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
@@ -34486,46 +34492,46 @@
       <c r="AC52" s="14"/>
     </row>
     <row r="53" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="30"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="16"/>
-      <c r="F53" s="19" t="s">
+      <c r="F53" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="21"/>
-      <c r="K53" s="28" t="s">
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="34"/>
+      <c r="K53" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="30"/>
+      <c r="L53" s="30"/>
+      <c r="M53" s="30"/>
+      <c r="N53" s="31"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="28" t="s">
+      <c r="P53" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="Q53" s="29"/>
-      <c r="R53" s="29"/>
-      <c r="S53" s="30"/>
+      <c r="Q53" s="30"/>
+      <c r="R53" s="30"/>
+      <c r="S53" s="31"/>
       <c r="T53" s="16"/>
-      <c r="U53" s="28" t="s">
+      <c r="U53" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="V53" s="29"/>
-      <c r="W53" s="29"/>
-      <c r="X53" s="30"/>
+      <c r="V53" s="30"/>
+      <c r="W53" s="30"/>
+      <c r="X53" s="31"/>
       <c r="Y53" s="16"/>
-      <c r="Z53" s="28" t="s">
+      <c r="Z53" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AA53" s="29"/>
-      <c r="AB53" s="29"/>
-      <c r="AC53" s="30"/>
+      <c r="AA53" s="30"/>
+      <c r="AB53" s="30"/>
+      <c r="AC53" s="31"/>
     </row>
     <row r="54" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -35009,33 +35015,33 @@
       <c r="I60" s="9">
         <v>0.26</v>
       </c>
-      <c r="K60" s="19" t="s">
+      <c r="K60" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L60" s="20"/>
-      <c r="M60" s="20"/>
-      <c r="N60" s="21"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="33"/>
+      <c r="N60" s="34"/>
       <c r="O60" s="16"/>
-      <c r="P60" s="19" t="s">
+      <c r="P60" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="Q60" s="20"/>
-      <c r="R60" s="20"/>
-      <c r="S60" s="21"/>
+      <c r="Q60" s="33"/>
+      <c r="R60" s="33"/>
+      <c r="S60" s="34"/>
       <c r="T60" s="16"/>
-      <c r="U60" s="19" t="s">
+      <c r="U60" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="V60" s="20"/>
-      <c r="W60" s="20"/>
-      <c r="X60" s="21"/>
+      <c r="V60" s="33"/>
+      <c r="W60" s="33"/>
+      <c r="X60" s="34"/>
       <c r="Y60" s="16"/>
-      <c r="Z60" s="19" t="s">
+      <c r="Z60" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="AA60" s="20"/>
-      <c r="AB60" s="20"/>
-      <c r="AC60" s="21"/>
+      <c r="AA60" s="33"/>
+      <c r="AB60" s="33"/>
+      <c r="AC60" s="34"/>
     </row>
     <row r="61" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -35527,20 +35533,18 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="AE5:AH5"/>
-    <mergeCell ref="AE1:AH2"/>
-    <mergeCell ref="P53:S53"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="P21:S21"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="U53:X53"/>
-    <mergeCell ref="Z53:AC53"/>
+    <mergeCell ref="P60:S60"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="Z37:AC37"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="Z44:AC44"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="U12:X12"/>
+    <mergeCell ref="Z12:AC12"/>
+    <mergeCell ref="U21:X21"/>
+    <mergeCell ref="Z21:AC21"/>
     <mergeCell ref="U60:X60"/>
     <mergeCell ref="Z60:AC60"/>
     <mergeCell ref="A1:I2"/>
@@ -35557,20 +35561,22 @@
     <mergeCell ref="K53:N53"/>
     <mergeCell ref="K60:N60"/>
     <mergeCell ref="P28:S28"/>
+    <mergeCell ref="AE5:AH5"/>
+    <mergeCell ref="AE1:AH2"/>
+    <mergeCell ref="P53:S53"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="P21:S21"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="U53:X53"/>
+    <mergeCell ref="Z53:AC53"/>
     <mergeCell ref="K1:AC2"/>
     <mergeCell ref="Z28:AC28"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="Z37:AC37"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="Z44:AC44"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="U12:X12"/>
-    <mergeCell ref="Z12:AC12"/>
-    <mergeCell ref="U21:X21"/>
-    <mergeCell ref="Z21:AC21"/>
-    <mergeCell ref="P60:S60"/>
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="U28:X28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Full Genetic Algorithm CNN Models
CNN, DenseNet, ResNet, and VGG models, ready to be tested for all 6 * 2 datasets
</commit_message>
<xml_diff>
--- a/preformance logs/Vectors/features/Performance Logs.xlsx
+++ b/preformance logs/Vectors/features/Performance Logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pana\Desktop\Northumbria\Final Year\Individual Computing Project KV6003BNN01\Speech-Emotion-Recognition---Audio-Dataset\preformance logs\Vectors\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3BE333-A801-4512-9584-EEDC9C03A0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3E7D7F-4B78-4D31-B8F3-91413B4897A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1620" windowWidth="21600" windowHeight="11835" xr2:uid="{61528B2F-A6A9-4B14-924A-8C83E0EA857F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{61528B2F-A6A9-4B14-924A-8C83E0EA857F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="76">
   <si>
     <t>ANN</t>
   </si>
@@ -214,12 +214,6 @@
     <t>SAVEE: MFCC  256X256</t>
   </si>
   <si>
-    <t>3 Channel Feature EMODB Dataset</t>
-  </si>
-  <si>
-    <t>Vector Features - Gen Alg Optimisation</t>
-  </si>
-  <si>
     <t>CH_ME_MF</t>
   </si>
   <si>
@@ -237,12 +231,48 @@
   <si>
     <t>ME_MF_CH</t>
   </si>
+  <si>
+    <t>3 Channel Feature EMODB Dataset 512x512</t>
+  </si>
+  <si>
+    <t>3 Channel Feature RAVDESS Dataset 512x512</t>
+  </si>
+  <si>
+    <t>3 Features Channel Images - Gen Alg Optimisation - 128x128</t>
+  </si>
+  <si>
+    <t>CNN - EMODB</t>
+  </si>
+  <si>
+    <t>CNN - RAVDESS</t>
+  </si>
+  <si>
+    <t>RESNET - EMODB</t>
+  </si>
+  <si>
+    <t>RESNET - RAVDESS</t>
+  </si>
+  <si>
+    <t>DENSENET - EMODB</t>
+  </si>
+  <si>
+    <t>DENSENET - RAVDESS</t>
+  </si>
+  <si>
+    <t>3 Features Channel Images - Gen Alg Optimisation - 128x128 - 4 CLASSES ONLY</t>
+  </si>
+  <si>
+    <t>VGG - EMODB</t>
+  </si>
+  <si>
+    <t>VGG - RAVDESS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,8 +311,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +408,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF5757"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEC7014"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB547"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCA7D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDDAB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -562,9 +624,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,10 +645,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -601,18 +702,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -622,13 +711,13 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,16 +728,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFDDAB"/>
+      <color rgb="FFFFCA7D"/>
+      <color rgb="FFFFBD5B"/>
+      <color rgb="FFFFB547"/>
+      <color rgb="FFEC7014"/>
       <color rgb="FFFF5757"/>
       <color rgb="FFFF9393"/>
       <color rgb="FFFF8989"/>
       <color rgb="FFFFD3D3"/>
       <color rgb="FFFF7979"/>
-      <color rgb="FFEC7014"/>
-      <color rgb="FFCB181D"/>
-      <color rgb="FF238B45"/>
-      <color rgb="FF2171B5"/>
-      <color rgb="FFFD9351"/>
     </mruColors>
   </colors>
   <extLst>
@@ -31103,10 +31192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E156107A-CEDE-4609-AC71-C70C41097B85}">
-  <dimension ref="A1:AM68"/>
+  <dimension ref="A1:BF68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AW39" sqref="AW39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31117,95 +31206,119 @@
     <col min="15" max="15" width="17.5703125" customWidth="1"/>
     <col min="16" max="29" width="18.5703125" customWidth="1"/>
     <col min="30" max="30" width="25.5703125" customWidth="1"/>
-    <col min="31" max="34" width="18.5703125" customWidth="1"/>
+    <col min="31" max="51" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="38"/>
-      <c r="AE1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="47"/>
+      <c r="AE1" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AP1" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="41"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
+    <row r="2" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="48"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AP2" s="36"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
     </row>
-    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -31235,8 +31348,32 @@
       <c r="AA3" s="16"/>
       <c r="AB3" s="16"/>
       <c r="AC3" s="14"/>
+      <c r="AE3" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="31"/>
+      <c r="AK3" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" s="31"/>
+      <c r="AM3" s="31"/>
+      <c r="AN3" s="31"/>
+      <c r="AP3" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ3" s="31"/>
+      <c r="AR3" s="31"/>
+      <c r="AS3" s="31"/>
+      <c r="AV3" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW3" s="31"/>
+      <c r="AX3" s="31"/>
+      <c r="AY3" s="31"/>
     </row>
-    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -31265,56 +31402,88 @@
       <c r="AA4" s="16"/>
       <c r="AB4" s="16"/>
       <c r="AC4" s="14"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AK4" s="31"/>
+      <c r="AL4" s="31"/>
+      <c r="AM4" s="31"/>
+      <c r="AN4" s="31"/>
+      <c r="AP4" s="31"/>
+      <c r="AQ4" s="31"/>
+      <c r="AR4" s="31"/>
+      <c r="AS4" s="31"/>
+      <c r="AV4" s="31"/>
+      <c r="AW4" s="31"/>
+      <c r="AX4" s="31"/>
+      <c r="AY4" s="31"/>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="16"/>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="K5" s="29" t="s">
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="K5" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="31"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="44"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="29" t="s">
+      <c r="P5" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="31"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="44"/>
       <c r="T5" s="16"/>
-      <c r="U5" s="29" t="s">
+      <c r="U5" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="31"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="44"/>
       <c r="Y5" s="16"/>
-      <c r="Z5" s="29" t="s">
+      <c r="Z5" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="31"/>
-      <c r="AE5" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="27"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="44"/>
+      <c r="AE5" s="32"/>
+      <c r="AF5" s="32"/>
+      <c r="AG5" s="32"/>
+      <c r="AH5" s="32"/>
+      <c r="AK5" s="32"/>
+      <c r="AL5" s="32"/>
+      <c r="AM5" s="32"/>
+      <c r="AN5" s="32"/>
+      <c r="AP5" s="32"/>
+      <c r="AQ5" s="32"/>
+      <c r="AR5" s="32"/>
+      <c r="AS5" s="32"/>
+      <c r="AV5" s="32"/>
+      <c r="AW5" s="32"/>
+      <c r="AX5" s="32"/>
+      <c r="AY5" s="32"/>
+      <c r="BC5" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD5" s="41"/>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -31379,18 +31548,58 @@
       <c r="AC6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="24" t="s">
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="AG6" s="24" t="s">
+      <c r="AG6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AH6" s="24" t="s">
+      <c r="AH6" s="23" t="s">
         <v>12</v>
       </c>
+      <c r="AK6" s="21"/>
+      <c r="AL6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP6" s="21"/>
+      <c r="AQ6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV6" s="21"/>
+      <c r="AW6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC6" s="21"/>
+      <c r="BD6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="BE6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF6" s="23" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -31467,20 +31676,44 @@
       <c r="AC7" s="10">
         <v>0.51</v>
       </c>
-      <c r="AE7" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF7" s="20">
+      <c r="AE7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="19"/>
+      <c r="AK7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL7" s="19"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="19"/>
+      <c r="AP7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ7" s="19"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="19"/>
+      <c r="AV7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW7" s="19"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="19"/>
+      <c r="BC7" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD7" s="19">
         <v>0.79</v>
       </c>
-      <c r="AG7" s="21">
+      <c r="BE7" s="20">
         <v>0.73</v>
       </c>
-      <c r="AH7" s="20">
+      <c r="BF7" s="19">
         <v>0.79</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -31557,20 +31790,44 @@
       <c r="AC8" s="10">
         <v>0.49</v>
       </c>
-      <c r="AE8" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF8" s="20">
+      <c r="AE8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="19"/>
+      <c r="AK8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL8" s="19"/>
+      <c r="AM8" s="20"/>
+      <c r="AN8" s="19"/>
+      <c r="AP8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ8" s="19"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="19"/>
+      <c r="AV8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW8" s="19"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="19"/>
+      <c r="BC8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="BD8" s="19">
         <v>0.78</v>
       </c>
-      <c r="AG8" s="21">
+      <c r="BE8" s="20">
         <v>0.7</v>
       </c>
-      <c r="AH8" s="20">
+      <c r="BF8" s="19">
         <v>0.77</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -31648,20 +31905,44 @@
       <c r="AC9" s="10">
         <v>0.5</v>
       </c>
-      <c r="AE9" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF9" s="20">
+      <c r="AE9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF9" s="19"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="19"/>
+      <c r="AK9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL9" s="19"/>
+      <c r="AM9" s="20"/>
+      <c r="AN9" s="19"/>
+      <c r="AP9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ9" s="19"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="19"/>
+      <c r="AV9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW9" s="19"/>
+      <c r="AX9" s="20"/>
+      <c r="AY9" s="19"/>
+      <c r="BC9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD9" s="19">
         <v>0.81</v>
       </c>
-      <c r="AG9" s="21">
+      <c r="BE9" s="20">
         <v>0.75</v>
       </c>
-      <c r="AH9" s="20">
+      <c r="BF9" s="19">
         <v>0.81</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -31738,20 +32019,44 @@
       <c r="AC10" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AE10" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF10" s="20">
+      <c r="AE10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="19"/>
+      <c r="AK10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL10" s="19"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="19"/>
+      <c r="AP10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ10" s="19"/>
+      <c r="AR10" s="20"/>
+      <c r="AS10" s="19"/>
+      <c r="AV10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW10" s="19"/>
+      <c r="AX10" s="20"/>
+      <c r="AY10" s="19"/>
+      <c r="BC10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD10" s="19">
         <v>0.79</v>
       </c>
-      <c r="AG10" s="21">
+      <c r="BE10" s="20">
         <v>0.69</v>
       </c>
-      <c r="AH10" s="20">
+      <c r="BF10" s="19">
         <v>0.77</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -31828,20 +32133,44 @@
       <c r="AC11" s="10">
         <v>0.49</v>
       </c>
-      <c r="AE11" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF11" s="20">
+      <c r="AE11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="20"/>
+      <c r="AH11" s="19"/>
+      <c r="AK11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL11" s="19"/>
+      <c r="AM11" s="20"/>
+      <c r="AN11" s="19"/>
+      <c r="AP11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ11" s="19"/>
+      <c r="AR11" s="20"/>
+      <c r="AS11" s="19"/>
+      <c r="AV11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW11" s="19"/>
+      <c r="AX11" s="20"/>
+      <c r="AY11" s="19"/>
+      <c r="BC11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD11" s="19">
         <v>0.74</v>
       </c>
-      <c r="AG11" s="21">
+      <c r="BE11" s="20">
         <v>0.66</v>
       </c>
-      <c r="AH11" s="20">
+      <c r="BF11" s="19">
         <v>0.73</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -31867,47 +32196,71 @@
       <c r="I12" s="9">
         <v>0.37</v>
       </c>
-      <c r="K12" s="32" t="s">
+      <c r="K12" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="34"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="40"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="32" t="s">
+      <c r="P12" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="34"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="40"/>
       <c r="T12" s="16"/>
-      <c r="U12" s="32" t="s">
+      <c r="U12" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="V12" s="33"/>
-      <c r="W12" s="33"/>
-      <c r="X12" s="34"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="40"/>
       <c r="Y12" s="16"/>
-      <c r="Z12" s="32" t="s">
+      <c r="Z12" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="AA12" s="33"/>
-      <c r="AB12" s="33"/>
-      <c r="AC12" s="34"/>
-      <c r="AE12" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF12" s="20">
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="40"/>
+      <c r="AE12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="19"/>
+      <c r="AK12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL12" s="19"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="19"/>
+      <c r="AP12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ12" s="19"/>
+      <c r="AR12" s="20"/>
+      <c r="AS12" s="19"/>
+      <c r="AV12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW12" s="19"/>
+      <c r="AX12" s="20"/>
+      <c r="AY12" s="19"/>
+      <c r="BC12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD12" s="19">
         <v>0.81</v>
       </c>
-      <c r="AG12" s="21">
+      <c r="BE12" s="20">
         <v>0.74</v>
       </c>
-      <c r="AH12" s="20">
+      <c r="BF12" s="19">
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -31976,12 +32329,36 @@
       <c r="AC13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AE13" s="25"/>
-      <c r="AF13" s="26"/>
-      <c r="AG13" s="26"/>
-      <c r="AH13" s="26"/>
+      <c r="AE13" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF13" s="33"/>
+      <c r="AG13" s="33"/>
+      <c r="AH13" s="33"/>
+      <c r="AK13" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL13" s="33"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="33"/>
+      <c r="AP13" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ13" s="33"/>
+      <c r="AR13" s="33"/>
+      <c r="AS13" s="33"/>
+      <c r="AV13" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW13" s="33"/>
+      <c r="AX13" s="33"/>
+      <c r="AY13" s="33"/>
+      <c r="BC13" s="24"/>
+      <c r="BD13" s="25"/>
+      <c r="BE13" s="25"/>
+      <c r="BF13" s="25"/>
     </row>
-    <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -32058,12 +32435,28 @@
       <c r="AC14" s="9">
         <v>0.04</v>
       </c>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="26"/>
+      <c r="AE14" s="34"/>
+      <c r="AF14" s="34"/>
+      <c r="AG14" s="34"/>
+      <c r="AH14" s="34"/>
+      <c r="AK14" s="34"/>
+      <c r="AL14" s="34"/>
+      <c r="AM14" s="34"/>
+      <c r="AN14" s="34"/>
+      <c r="AP14" s="34"/>
+      <c r="AQ14" s="34"/>
+      <c r="AR14" s="34"/>
+      <c r="AS14" s="34"/>
+      <c r="AV14" s="34"/>
+      <c r="AW14" s="34"/>
+      <c r="AX14" s="34"/>
+      <c r="AY14" s="34"/>
+      <c r="BC14" s="24"/>
+      <c r="BD14" s="25"/>
+      <c r="BE14" s="25"/>
+      <c r="BF14" s="25"/>
     </row>
-    <row r="15" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -32140,12 +32533,30 @@
       <c r="AC15" s="9">
         <v>0.43</v>
       </c>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="26"/>
-      <c r="AG15" s="26"/>
-      <c r="AH15" s="26"/>
+      <c r="AE15" s="35"/>
+      <c r="AF15" s="35"/>
+      <c r="AG15" s="35"/>
+      <c r="AH15" s="35"/>
+      <c r="AK15" s="35"/>
+      <c r="AL15" s="35"/>
+      <c r="AM15" s="35"/>
+      <c r="AN15" s="35"/>
+      <c r="AP15" s="35"/>
+      <c r="AQ15" s="35"/>
+      <c r="AR15" s="35"/>
+      <c r="AS15" s="35"/>
+      <c r="AV15" s="35"/>
+      <c r="AW15" s="35"/>
+      <c r="AX15" s="35"/>
+      <c r="AY15" s="35"/>
+      <c r="BC15" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD15" s="41"/>
+      <c r="BE15" s="41"/>
+      <c r="BF15" s="41"/>
     </row>
-    <row r="16" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -32222,12 +32633,58 @@
       <c r="AC16" s="9">
         <v>0.4</v>
       </c>
-      <c r="AE16" s="25"/>
-      <c r="AF16" s="26"/>
-      <c r="AG16" s="26"/>
-      <c r="AH16" s="26"/>
+      <c r="AE16" s="26"/>
+      <c r="AF16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK16" s="26"/>
+      <c r="AL16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP16" s="26"/>
+      <c r="AQ16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV16" s="26"/>
+      <c r="AW16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC16" s="21"/>
+      <c r="BD16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="BE16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF16" s="23" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -32288,8 +32745,44 @@
       <c r="AC17" s="9">
         <v>0.48</v>
       </c>
+      <c r="AE17" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="30"/>
+      <c r="AK17" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="29"/>
+      <c r="AN17" s="30"/>
+      <c r="AP17" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ17" s="30"/>
+      <c r="AR17" s="29"/>
+      <c r="AS17" s="30"/>
+      <c r="AV17" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW17" s="30"/>
+      <c r="AX17" s="29"/>
+      <c r="AY17" s="30"/>
+      <c r="BC17" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD17" s="19">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="BE17" s="20">
+        <v>0.54</v>
+      </c>
+      <c r="BF17" s="19">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -32350,8 +32843,44 @@
       <c r="AC18" s="9">
         <v>0.44</v>
       </c>
+      <c r="AE18" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF18" s="30"/>
+      <c r="AG18" s="29"/>
+      <c r="AH18" s="30"/>
+      <c r="AK18" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL18" s="30"/>
+      <c r="AM18" s="29"/>
+      <c r="AN18" s="30"/>
+      <c r="AP18" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ18" s="30"/>
+      <c r="AR18" s="29"/>
+      <c r="AS18" s="30"/>
+      <c r="AV18" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW18" s="30"/>
+      <c r="AX18" s="29"/>
+      <c r="AY18" s="30"/>
+      <c r="BC18" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="BD18" s="19">
+        <v>0.59</v>
+      </c>
+      <c r="BE18" s="20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="BF18" s="19">
+        <v>0.59</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -32380,8 +32909,44 @@
       <c r="AA19" s="16"/>
       <c r="AB19" s="16"/>
       <c r="AC19" s="14"/>
+      <c r="AE19" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF19" s="30"/>
+      <c r="AG19" s="29"/>
+      <c r="AH19" s="30"/>
+      <c r="AK19" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL19" s="30"/>
+      <c r="AM19" s="29"/>
+      <c r="AN19" s="30"/>
+      <c r="AP19" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ19" s="30"/>
+      <c r="AR19" s="29"/>
+      <c r="AS19" s="30"/>
+      <c r="AV19" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW19" s="30"/>
+      <c r="AX19" s="29"/>
+      <c r="AY19" s="30"/>
+      <c r="BC19" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD19" s="19">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="BE19" s="20">
+        <v>0.54</v>
+      </c>
+      <c r="BF19" s="19">
+        <v>0.56000000000000005</v>
+      </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -32410,50 +32975,116 @@
       <c r="AA20" s="16"/>
       <c r="AB20" s="16"/>
       <c r="AC20" s="14"/>
+      <c r="AE20" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF20" s="30"/>
+      <c r="AG20" s="29"/>
+      <c r="AH20" s="30"/>
+      <c r="AK20" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL20" s="30"/>
+      <c r="AM20" s="29"/>
+      <c r="AN20" s="30"/>
+      <c r="AP20" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ20" s="30"/>
+      <c r="AR20" s="29"/>
+      <c r="AS20" s="30"/>
+      <c r="AV20" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW20" s="30"/>
+      <c r="AX20" s="29"/>
+      <c r="AY20" s="30"/>
+      <c r="BC20" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="BD20" s="19"/>
+      <c r="BE20" s="20"/>
+      <c r="BF20" s="19"/>
     </row>
-    <row r="21" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="34"/>
-      <c r="K21" s="29" t="s">
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
+      <c r="K21" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="31"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="29" t="s">
+      <c r="P21" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="31"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="44"/>
       <c r="T21" s="16"/>
-      <c r="U21" s="29" t="s">
+      <c r="U21" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="31"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="44"/>
       <c r="Y21" s="16"/>
-      <c r="Z21" s="29" t="s">
+      <c r="Z21" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="AA21" s="30"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="31"/>
+      <c r="AA21" s="43"/>
+      <c r="AB21" s="43"/>
+      <c r="AC21" s="44"/>
+      <c r="AE21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF21" s="30"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="30"/>
+      <c r="AK21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL21" s="30"/>
+      <c r="AM21" s="29"/>
+      <c r="AN21" s="30"/>
+      <c r="AP21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ21" s="30"/>
+      <c r="AR21" s="29"/>
+      <c r="AS21" s="30"/>
+      <c r="AV21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW21" s="30"/>
+      <c r="AX21" s="29"/>
+      <c r="AY21" s="30"/>
+      <c r="BC21" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD21" s="19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="BE21" s="20">
+        <v>0.53</v>
+      </c>
+      <c r="BF21" s="19">
+        <v>0.54</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
         <v>10</v>
@@ -32518,8 +33149,44 @@
       <c r="AC22" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AE22" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF22" s="30"/>
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="30"/>
+      <c r="AK22" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL22" s="30"/>
+      <c r="AM22" s="29"/>
+      <c r="AN22" s="30"/>
+      <c r="AP22" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ22" s="30"/>
+      <c r="AR22" s="29"/>
+      <c r="AS22" s="30"/>
+      <c r="AV22" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW22" s="30"/>
+      <c r="AX22" s="29"/>
+      <c r="AY22" s="30"/>
+      <c r="BC22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD22" s="19">
+        <v>0.62</v>
+      </c>
+      <c r="BE22" s="20">
+        <v>0.62</v>
+      </c>
+      <c r="BF22" s="19">
+        <v>0.62</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
@@ -32596,8 +33263,32 @@
       <c r="AC23" s="10">
         <v>0.61</v>
       </c>
+      <c r="AE23" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF23" s="31"/>
+      <c r="AG23" s="31"/>
+      <c r="AH23" s="31"/>
+      <c r="AK23" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL23" s="31"/>
+      <c r="AM23" s="31"/>
+      <c r="AN23" s="31"/>
+      <c r="AP23" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ23" s="31"/>
+      <c r="AR23" s="31"/>
+      <c r="AS23" s="31"/>
+      <c r="AV23" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW23" s="31"/>
+      <c r="AX23" s="31"/>
+      <c r="AY23" s="31"/>
     </row>
-    <row r="24" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
@@ -32674,8 +33365,24 @@
       <c r="AC24" s="10">
         <v>0.74</v>
       </c>
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+      <c r="AG24" s="31"/>
+      <c r="AH24" s="31"/>
+      <c r="AK24" s="31"/>
+      <c r="AL24" s="31"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="31"/>
+      <c r="AP24" s="31"/>
+      <c r="AQ24" s="31"/>
+      <c r="AR24" s="31"/>
+      <c r="AS24" s="31"/>
+      <c r="AV24" s="31"/>
+      <c r="AW24" s="31"/>
+      <c r="AX24" s="31"/>
+      <c r="AY24" s="31"/>
     </row>
-    <row r="25" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>2</v>
       </c>
@@ -32752,8 +33459,24 @@
       <c r="AC25" s="10">
         <v>0.71</v>
       </c>
+      <c r="AE25" s="32"/>
+      <c r="AF25" s="32"/>
+      <c r="AG25" s="32"/>
+      <c r="AH25" s="32"/>
+      <c r="AK25" s="32"/>
+      <c r="AL25" s="32"/>
+      <c r="AM25" s="32"/>
+      <c r="AN25" s="32"/>
+      <c r="AP25" s="32"/>
+      <c r="AQ25" s="32"/>
+      <c r="AR25" s="32"/>
+      <c r="AS25" s="32"/>
+      <c r="AV25" s="32"/>
+      <c r="AW25" s="32"/>
+      <c r="AX25" s="32"/>
+      <c r="AY25" s="32"/>
     </row>
-    <row r="26" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
@@ -32830,8 +33553,48 @@
       <c r="AC26" s="10">
         <v>0.66</v>
       </c>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH26" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN26" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP26" s="21"/>
+      <c r="AQ26" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS26" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV26" s="21"/>
+      <c r="AW26" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY26" s="23" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
@@ -32908,8 +33671,32 @@
       <c r="AC27" s="10">
         <v>0.74</v>
       </c>
+      <c r="AE27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF27" s="19"/>
+      <c r="AG27" s="20"/>
+      <c r="AH27" s="19"/>
+      <c r="AK27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="20"/>
+      <c r="AN27" s="19"/>
+      <c r="AP27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ27" s="19"/>
+      <c r="AR27" s="20"/>
+      <c r="AS27" s="19"/>
+      <c r="AV27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW27" s="19"/>
+      <c r="AX27" s="20"/>
+      <c r="AY27" s="19"/>
     </row>
-    <row r="28" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
@@ -32935,35 +33722,59 @@
       <c r="I28" s="9">
         <v>0.24</v>
       </c>
-      <c r="K28" s="32" t="s">
+      <c r="K28" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="34"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="40"/>
       <c r="O28" s="16"/>
-      <c r="P28" s="32" t="s">
+      <c r="P28" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="34"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="40"/>
       <c r="T28" s="16"/>
-      <c r="U28" s="32" t="s">
+      <c r="U28" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="34"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="40"/>
       <c r="Y28" s="16"/>
-      <c r="Z28" s="32" t="s">
+      <c r="Z28" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="AA28" s="33"/>
-      <c r="AB28" s="33"/>
-      <c r="AC28" s="34"/>
+      <c r="AA28" s="39"/>
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="40"/>
+      <c r="AE28" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="20"/>
+      <c r="AH28" s="19"/>
+      <c r="AK28" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL28" s="19"/>
+      <c r="AM28" s="20"/>
+      <c r="AN28" s="19"/>
+      <c r="AP28" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ28" s="19"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="19"/>
+      <c r="AV28" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW28" s="19"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="19"/>
     </row>
-    <row r="29" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -33032,8 +33843,32 @@
       <c r="AC29" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="AE29" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="20"/>
+      <c r="AH29" s="19"/>
+      <c r="AK29" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL29" s="19"/>
+      <c r="AM29" s="20"/>
+      <c r="AN29" s="19"/>
+      <c r="AP29" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="19"/>
+      <c r="AV29" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW29" s="19"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="19"/>
     </row>
-    <row r="30" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
@@ -33110,8 +33945,32 @@
       <c r="AC30" s="9">
         <v>0.43</v>
       </c>
+      <c r="AE30" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF30" s="19"/>
+      <c r="AG30" s="20"/>
+      <c r="AH30" s="19"/>
+      <c r="AK30" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL30" s="19"/>
+      <c r="AM30" s="20"/>
+      <c r="AN30" s="19"/>
+      <c r="AP30" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ30" s="19"/>
+      <c r="AR30" s="20"/>
+      <c r="AS30" s="19"/>
+      <c r="AV30" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW30" s="19"/>
+      <c r="AX30" s="20"/>
+      <c r="AY30" s="19"/>
     </row>
-    <row r="31" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
@@ -33188,8 +34047,32 @@
       <c r="AC31" s="9">
         <v>0.74</v>
       </c>
+      <c r="AE31" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="20"/>
+      <c r="AH31" s="19"/>
+      <c r="AK31" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL31" s="19"/>
+      <c r="AM31" s="20"/>
+      <c r="AN31" s="19"/>
+      <c r="AP31" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ31" s="19"/>
+      <c r="AR31" s="20"/>
+      <c r="AS31" s="19"/>
+      <c r="AV31" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW31" s="19"/>
+      <c r="AX31" s="20"/>
+      <c r="AY31" s="19"/>
     </row>
-    <row r="32" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
@@ -33266,8 +34149,32 @@
       <c r="AC32" s="9">
         <v>0.6</v>
       </c>
+      <c r="AE32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF32" s="19"/>
+      <c r="AG32" s="20"/>
+      <c r="AH32" s="19"/>
+      <c r="AK32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL32" s="19"/>
+      <c r="AM32" s="20"/>
+      <c r="AN32" s="19"/>
+      <c r="AP32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ32" s="19"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="19"/>
+      <c r="AV32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW32" s="19"/>
+      <c r="AX32" s="20"/>
+      <c r="AY32" s="19"/>
     </row>
-    <row r="33" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -33328,8 +34235,32 @@
       <c r="AC33" s="9">
         <v>0.61</v>
       </c>
+      <c r="AE33" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF33" s="33"/>
+      <c r="AG33" s="33"/>
+      <c r="AH33" s="33"/>
+      <c r="AK33" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL33" s="33"/>
+      <c r="AM33" s="33"/>
+      <c r="AN33" s="33"/>
+      <c r="AP33" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ33" s="33"/>
+      <c r="AR33" s="33"/>
+      <c r="AS33" s="33"/>
+      <c r="AV33" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW33" s="33"/>
+      <c r="AX33" s="33"/>
+      <c r="AY33" s="33"/>
     </row>
-    <row r="34" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -33390,8 +34321,24 @@
       <c r="AC34" s="9">
         <v>0.69</v>
       </c>
+      <c r="AE34" s="34"/>
+      <c r="AF34" s="34"/>
+      <c r="AG34" s="34"/>
+      <c r="AH34" s="34"/>
+      <c r="AK34" s="34"/>
+      <c r="AL34" s="34"/>
+      <c r="AM34" s="34"/>
+      <c r="AN34" s="34"/>
+      <c r="AP34" s="34"/>
+      <c r="AQ34" s="34"/>
+      <c r="AR34" s="34"/>
+      <c r="AS34" s="34"/>
+      <c r="AV34" s="34"/>
+      <c r="AW34" s="34"/>
+      <c r="AX34" s="34"/>
+      <c r="AY34" s="34"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -33420,8 +34367,24 @@
       <c r="AA35" s="16"/>
       <c r="AB35" s="16"/>
       <c r="AC35" s="14"/>
+      <c r="AE35" s="35"/>
+      <c r="AF35" s="35"/>
+      <c r="AG35" s="35"/>
+      <c r="AH35" s="35"/>
+      <c r="AK35" s="35"/>
+      <c r="AL35" s="35"/>
+      <c r="AM35" s="35"/>
+      <c r="AN35" s="35"/>
+      <c r="AP35" s="35"/>
+      <c r="AQ35" s="35"/>
+      <c r="AR35" s="35"/>
+      <c r="AS35" s="35"/>
+      <c r="AV35" s="35"/>
+      <c r="AW35" s="35"/>
+      <c r="AX35" s="35"/>
+      <c r="AY35" s="35"/>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -33450,50 +34413,114 @@
       <c r="AA36" s="16"/>
       <c r="AB36" s="16"/>
       <c r="AC36" s="14"/>
+      <c r="AE36" s="26"/>
+      <c r="AF36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH36" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK36" s="26"/>
+      <c r="AL36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN36" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP36" s="26"/>
+      <c r="AQ36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS36" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV36" s="26"/>
+      <c r="AW36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY36" s="28" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="37" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+    <row r="37" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
       <c r="E37" s="16"/>
-      <c r="F37" s="32" t="s">
+      <c r="F37" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="34"/>
-      <c r="K37" s="29" t="s">
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="40"/>
+      <c r="K37" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="31"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="44"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="29" t="s">
+      <c r="P37" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="31"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="43"/>
+      <c r="S37" s="44"/>
       <c r="T37" s="16"/>
-      <c r="U37" s="29" t="s">
+      <c r="U37" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="31"/>
+      <c r="V37" s="43"/>
+      <c r="W37" s="43"/>
+      <c r="X37" s="44"/>
       <c r="Y37" s="16"/>
-      <c r="Z37" s="29" t="s">
+      <c r="Z37" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="AA37" s="30"/>
-      <c r="AB37" s="30"/>
-      <c r="AC37" s="31"/>
+      <c r="AA37" s="43"/>
+      <c r="AB37" s="43"/>
+      <c r="AC37" s="44"/>
+      <c r="AE37" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF37" s="30"/>
+      <c r="AG37" s="29"/>
+      <c r="AH37" s="30"/>
+      <c r="AK37" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL37" s="30"/>
+      <c r="AM37" s="29"/>
+      <c r="AN37" s="30"/>
+      <c r="AP37" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ37" s="30"/>
+      <c r="AR37" s="29"/>
+      <c r="AS37" s="30"/>
+      <c r="AV37" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW37" s="30"/>
+      <c r="AX37" s="29"/>
+      <c r="AY37" s="30"/>
     </row>
-    <row r="38" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
         <v>10</v>
@@ -33558,8 +34585,32 @@
       <c r="AC38" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AE38" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF38" s="30"/>
+      <c r="AG38" s="29"/>
+      <c r="AH38" s="30"/>
+      <c r="AK38" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL38" s="30"/>
+      <c r="AM38" s="29"/>
+      <c r="AN38" s="30"/>
+      <c r="AP38" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ38" s="30"/>
+      <c r="AR38" s="29"/>
+      <c r="AS38" s="30"/>
+      <c r="AV38" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW38" s="30"/>
+      <c r="AX38" s="29"/>
+      <c r="AY38" s="30"/>
     </row>
-    <row r="39" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -33636,8 +34687,32 @@
       <c r="AC39" s="10">
         <v>0.61</v>
       </c>
+      <c r="AE39" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF39" s="30"/>
+      <c r="AG39" s="29"/>
+      <c r="AH39" s="30"/>
+      <c r="AK39" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL39" s="30"/>
+      <c r="AM39" s="29"/>
+      <c r="AN39" s="30"/>
+      <c r="AP39" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ39" s="30"/>
+      <c r="AR39" s="29"/>
+      <c r="AS39" s="30"/>
+      <c r="AV39" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW39" s="30"/>
+      <c r="AX39" s="29"/>
+      <c r="AY39" s="30"/>
     </row>
-    <row r="40" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>1</v>
       </c>
@@ -33714,8 +34789,32 @@
       <c r="AC40" s="10">
         <v>0.6</v>
       </c>
+      <c r="AE40" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF40" s="30"/>
+      <c r="AG40" s="29"/>
+      <c r="AH40" s="30"/>
+      <c r="AK40" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL40" s="30"/>
+      <c r="AM40" s="29"/>
+      <c r="AN40" s="30"/>
+      <c r="AP40" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ40" s="30"/>
+      <c r="AR40" s="29"/>
+      <c r="AS40" s="30"/>
+      <c r="AV40" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW40" s="30"/>
+      <c r="AX40" s="29"/>
+      <c r="AY40" s="30"/>
     </row>
-    <row r="41" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>2</v>
       </c>
@@ -33792,8 +34891,32 @@
       <c r="AC41" s="10">
         <v>0.54</v>
       </c>
+      <c r="AE41" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF41" s="30"/>
+      <c r="AG41" s="29"/>
+      <c r="AH41" s="30"/>
+      <c r="AK41" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL41" s="30"/>
+      <c r="AM41" s="29"/>
+      <c r="AN41" s="30"/>
+      <c r="AP41" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ41" s="30"/>
+      <c r="AR41" s="29"/>
+      <c r="AS41" s="30"/>
+      <c r="AV41" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW41" s="30"/>
+      <c r="AX41" s="29"/>
+      <c r="AY41" s="30"/>
     </row>
-    <row r="42" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>3</v>
       </c>
@@ -33870,8 +34993,32 @@
       <c r="AC42" s="10">
         <v>0.66</v>
       </c>
+      <c r="AE42" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF42" s="30"/>
+      <c r="AG42" s="29"/>
+      <c r="AH42" s="30"/>
+      <c r="AK42" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL42" s="30"/>
+      <c r="AM42" s="29"/>
+      <c r="AN42" s="30"/>
+      <c r="AP42" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ42" s="30"/>
+      <c r="AR42" s="29"/>
+      <c r="AS42" s="30"/>
+      <c r="AV42" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW42" s="30"/>
+      <c r="AX42" s="29"/>
+      <c r="AY42" s="30"/>
     </row>
-    <row r="43" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>4</v>
       </c>
@@ -33949,7 +35096,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>5</v>
       </c>
@@ -33975,35 +35122,35 @@
       <c r="I44" s="9">
         <v>0.21</v>
       </c>
-      <c r="K44" s="32" t="s">
+      <c r="K44" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="34"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="40"/>
       <c r="O44" s="16"/>
-      <c r="P44" s="32" t="s">
+      <c r="P44" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="Q44" s="33"/>
-      <c r="R44" s="33"/>
-      <c r="S44" s="34"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="39"/>
+      <c r="S44" s="40"/>
       <c r="T44" s="16"/>
-      <c r="U44" s="32" t="s">
+      <c r="U44" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="V44" s="33"/>
-      <c r="W44" s="33"/>
-      <c r="X44" s="34"/>
+      <c r="V44" s="39"/>
+      <c r="W44" s="39"/>
+      <c r="X44" s="40"/>
       <c r="Y44" s="16"/>
-      <c r="Z44" s="32" t="s">
+      <c r="Z44" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="AA44" s="33"/>
-      <c r="AB44" s="33"/>
-      <c r="AC44" s="34"/>
+      <c r="AA44" s="39"/>
+      <c r="AB44" s="39"/>
+      <c r="AC44" s="40"/>
     </row>
-    <row r="45" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>6</v>
       </c>
@@ -34073,7 +35220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -34151,7 +35298,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
@@ -34229,7 +35376,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:51" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>9</v>
       </c>
@@ -34492,46 +35639,46 @@
       <c r="AC52" s="14"/>
     </row>
     <row r="53" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="31"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="44"/>
       <c r="E53" s="16"/>
-      <c r="F53" s="32" t="s">
+      <c r="F53" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="34"/>
-      <c r="K53" s="29" t="s">
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="40"/>
+      <c r="K53" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="L53" s="30"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="31"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
+      <c r="N53" s="44"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="29" t="s">
+      <c r="P53" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
-      <c r="S53" s="31"/>
+      <c r="Q53" s="43"/>
+      <c r="R53" s="43"/>
+      <c r="S53" s="44"/>
       <c r="T53" s="16"/>
-      <c r="U53" s="29" t="s">
+      <c r="U53" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="V53" s="30"/>
-      <c r="W53" s="30"/>
-      <c r="X53" s="31"/>
+      <c r="V53" s="43"/>
+      <c r="W53" s="43"/>
+      <c r="X53" s="44"/>
       <c r="Y53" s="16"/>
-      <c r="Z53" s="29" t="s">
+      <c r="Z53" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="AA53" s="30"/>
-      <c r="AB53" s="30"/>
-      <c r="AC53" s="31"/>
+      <c r="AA53" s="43"/>
+      <c r="AB53" s="43"/>
+      <c r="AC53" s="44"/>
     </row>
     <row r="54" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -35015,33 +36162,33 @@
       <c r="I60" s="9">
         <v>0.26</v>
       </c>
-      <c r="K60" s="32" t="s">
+      <c r="K60" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="34"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="40"/>
       <c r="O60" s="16"/>
-      <c r="P60" s="32" t="s">
+      <c r="P60" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="Q60" s="33"/>
-      <c r="R60" s="33"/>
-      <c r="S60" s="34"/>
+      <c r="Q60" s="39"/>
+      <c r="R60" s="39"/>
+      <c r="S60" s="40"/>
       <c r="T60" s="16"/>
-      <c r="U60" s="32" t="s">
+      <c r="U60" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="V60" s="33"/>
-      <c r="W60" s="33"/>
-      <c r="X60" s="34"/>
+      <c r="V60" s="39"/>
+      <c r="W60" s="39"/>
+      <c r="X60" s="40"/>
       <c r="Y60" s="16"/>
-      <c r="Z60" s="32" t="s">
+      <c r="Z60" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="AA60" s="33"/>
-      <c r="AB60" s="33"/>
-      <c r="AC60" s="34"/>
+      <c r="AA60" s="39"/>
+      <c r="AB60" s="39"/>
+      <c r="AC60" s="40"/>
     </row>
     <row r="61" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -35532,21 +36679,7 @@
       <c r="AC68" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="P60:S60"/>
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="Z37:AC37"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="Z44:AC44"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="U12:X12"/>
-    <mergeCell ref="Z12:AC12"/>
-    <mergeCell ref="U21:X21"/>
-    <mergeCell ref="Z21:AC21"/>
-    <mergeCell ref="U60:X60"/>
-    <mergeCell ref="Z60:AC60"/>
+  <mergeCells count="62">
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="F53:I53"/>
     <mergeCell ref="F37:I37"/>
@@ -35561,22 +36694,54 @@
     <mergeCell ref="K53:N53"/>
     <mergeCell ref="K60:N60"/>
     <mergeCell ref="P28:S28"/>
-    <mergeCell ref="AE5:AH5"/>
-    <mergeCell ref="AE1:AH2"/>
+    <mergeCell ref="P60:S60"/>
     <mergeCell ref="P53:S53"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="U60:X60"/>
+    <mergeCell ref="Z60:AC60"/>
+    <mergeCell ref="BC15:BF15"/>
+    <mergeCell ref="BC5:BF5"/>
+    <mergeCell ref="U53:X53"/>
+    <mergeCell ref="Z53:AC53"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="Z37:AC37"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="Z44:AC44"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="U12:X12"/>
+    <mergeCell ref="Z12:AC12"/>
+    <mergeCell ref="U21:X21"/>
+    <mergeCell ref="AK33:AN35"/>
+    <mergeCell ref="AE23:AH25"/>
+    <mergeCell ref="AE33:AH35"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="AE1:AN2"/>
+    <mergeCell ref="K1:AC2"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="P5:S5"/>
     <mergeCell ref="K21:N21"/>
     <mergeCell ref="P21:S21"/>
     <mergeCell ref="K12:N12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="U53:X53"/>
-    <mergeCell ref="Z53:AC53"/>
-    <mergeCell ref="K1:AC2"/>
+    <mergeCell ref="Z21:AC21"/>
     <mergeCell ref="Z28:AC28"/>
+    <mergeCell ref="AE3:AH5"/>
+    <mergeCell ref="AE13:AH15"/>
+    <mergeCell ref="AK3:AN5"/>
+    <mergeCell ref="AK13:AN15"/>
+    <mergeCell ref="AK23:AN25"/>
+    <mergeCell ref="AP23:AS25"/>
+    <mergeCell ref="AV23:AY25"/>
+    <mergeCell ref="AP33:AS35"/>
+    <mergeCell ref="AV33:AY35"/>
+    <mergeCell ref="AP1:AY2"/>
+    <mergeCell ref="AP3:AS5"/>
+    <mergeCell ref="AV3:AY5"/>
+    <mergeCell ref="AP13:AS15"/>
+    <mergeCell ref="AV13:AY15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>